<commit_message>
Actualizar saas_data.xlsx con datos más recientes
</commit_message>
<xml_diff>
--- a/public/data/saas_data.xlsx
+++ b/public/data/saas_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rzarroca\Documents\javascript\dashboard_financiero\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB16D860-5BE6-49C4-9B0B-1CD1E93E938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C3D3FA-23E9-4F2C-A376-FCFDE81A4153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3B440274-B911-42C7-92AE-162AB4111442}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="sample-saas-data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'sample-saas-data'!$A$1:$K$7</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'sample-saas-data'!$A$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -82,22 +82,25 @@
     <t>contraction</t>
   </si>
   <si>
-    <t>ene-24</t>
-  </si>
-  <si>
-    <t>feb-24</t>
-  </si>
-  <si>
-    <t>mar-24</t>
-  </si>
-  <si>
-    <t>abr-24</t>
-  </si>
-  <si>
-    <t>may-24</t>
-  </si>
-  <si>
-    <t>jun-24</t>
+    <t>enero</t>
+  </si>
+  <si>
+    <t>febrero</t>
+  </si>
+  <si>
+    <t>marzo</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
+  <si>
+    <t>mayo</t>
+  </si>
+  <si>
+    <t>junio</t>
+  </si>
+  <si>
+    <t>julio</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +130,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,12 +163,18 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -168,7 +183,8 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -189,10 +205,10 @@
       <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -231,20 +247,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2768432B-9119-48BB-9B4F-CA46E7F95CDF}" name="sample_saas_data" displayName="sample_saas_data" ref="A1:K7" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:K7" xr:uid="{2768432B-9119-48BB-9B4F-CA46E7F95CDF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2768432B-9119-48BB-9B4F-CA46E7F95CDF}" name="sample_saas_data" displayName="sample_saas_data" ref="A1:K8" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:K8" xr:uid="{2768432B-9119-48BB-9B4F-CA46E7F95CDF}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C45C579C-69B0-434B-8DC0-110FFB76C466}" uniqueName="1" name="date" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{547031ED-6B61-4AE6-A634-6120625C7426}" uniqueName="2" name="monthYear" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C5090219-89FB-48B7-A171-6A50DC4ED15D}" uniqueName="3" name="arr" queryTableFieldId="3" dataDxfId="1" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{360B8532-28F2-488E-9E6F-C2688F561A3B}" uniqueName="4" name="momGrowth" queryTableFieldId="4" dataDxfId="0" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{547031ED-6B61-4AE6-A634-6120625C7426}" uniqueName="2" name="monthYear" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C5090219-89FB-48B7-A171-6A50DC4ED15D}" uniqueName="3" name="arr" queryTableFieldId="3" dataDxfId="8" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{360B8532-28F2-488E-9E6F-C2688F561A3B}" uniqueName="4" name="momGrowth" queryTableFieldId="4" dataDxfId="7" dataCellStyle="Porcentaje"/>
     <tableColumn id="5" xr3:uid="{6EC1391E-177B-4B62-A924-CE5C6C5E3B4B}" uniqueName="5" name="customers" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{A3981157-ACC6-4E32-96C4-08C526FF69B2}" uniqueName="6" name="arpa" queryTableFieldId="6" dataDxfId="7" dataCellStyle="Moneda"/>
-    <tableColumn id="7" xr3:uid="{571477D1-1736-4CC2-BBD7-DE1F904FDE2F}" uniqueName="7" name="new" queryTableFieldId="7" dataDxfId="6" dataCellStyle="Moneda"/>
-    <tableColumn id="8" xr3:uid="{E6F32B3A-0B10-4E84-A26F-94C6FF1182E3}" uniqueName="8" name="expansion" queryTableFieldId="8" dataDxfId="5" dataCellStyle="Moneda"/>
-    <tableColumn id="9" xr3:uid="{E2DA2514-16FB-4D84-A8A2-C73229565805}" uniqueName="9" name="reactivation" queryTableFieldId="9" dataDxfId="4" dataCellStyle="Moneda"/>
-    <tableColumn id="10" xr3:uid="{027ED5D9-67F7-400B-8115-2DC46CE0B319}" uniqueName="10" name="churn" queryTableFieldId="10" dataDxfId="3" dataCellStyle="Moneda"/>
-    <tableColumn id="11" xr3:uid="{00BBEE66-5029-4715-9519-CCFCEB113583}" uniqueName="11" name="contraction" queryTableFieldId="11" dataDxfId="2" dataCellStyle="Moneda"/>
+    <tableColumn id="6" xr3:uid="{A3981157-ACC6-4E32-96C4-08C526FF69B2}" uniqueName="6" name="arpa" queryTableFieldId="6" dataDxfId="6" dataCellStyle="Moneda"/>
+    <tableColumn id="7" xr3:uid="{571477D1-1736-4CC2-BBD7-DE1F904FDE2F}" uniqueName="7" name="new" queryTableFieldId="7" dataDxfId="5" dataCellStyle="Moneda"/>
+    <tableColumn id="8" xr3:uid="{E6F32B3A-0B10-4E84-A26F-94C6FF1182E3}" uniqueName="8" name="expansion" queryTableFieldId="8" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="9" xr3:uid="{E2DA2514-16FB-4D84-A8A2-C73229565805}" uniqueName="9" name="reactivation" queryTableFieldId="9" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="10" xr3:uid="{027ED5D9-67F7-400B-8115-2DC46CE0B319}" uniqueName="10" name="churn" queryTableFieldId="10" dataDxfId="2" dataCellStyle="Moneda"/>
+    <tableColumn id="11" xr3:uid="{00BBEE66-5029-4715-9519-CCFCEB113583}" uniqueName="11" name="contraction" queryTableFieldId="11" dataDxfId="1" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -570,7 +586,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +642,7 @@
       <c r="A2" s="1">
         <v>45292</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2">
@@ -661,7 +677,7 @@
       <c r="A3" s="1">
         <v>45323</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2">
@@ -697,7 +713,7 @@
       <c r="A4" s="1">
         <v>45352</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2">
@@ -733,7 +749,7 @@
       <c r="A5" s="1">
         <v>45383</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2">
@@ -769,7 +785,7 @@
       <c r="A6" s="1">
         <v>45413</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2">
@@ -805,7 +821,7 @@
       <c r="A7" s="1">
         <v>45444</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="2">
@@ -836,11 +852,61 @@
       <c r="K7" s="2">
         <v>-10000</v>
       </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45474</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4500000</v>
+      </c>
+      <c r="D8" s="4">
+        <f>(sample_saas_data[[#This Row],[arr]]-C7)/C7*100</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="E8">
+        <v>230</v>
+      </c>
+      <c r="F8" s="2">
+        <f>sample_saas_data[[#This Row],[arr]]/sample_saas_data[[#This Row],[customers]]</f>
+        <v>19565.217391304348</v>
+      </c>
+      <c r="G8" s="2">
+        <v>50000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>43000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>9000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-20000</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-9000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F12" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>